<commit_message>
Platform ready for evaluation
</commit_message>
<xml_diff>
--- a/Assignment2/Instruction set.xlsx
+++ b/Assignment2/Instruction set.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
-  <si>
-    <t>LOAD</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>ADD</t>
   </si>
@@ -35,9 +32,6 @@
     <t xml:space="preserve">SUB </t>
   </si>
   <si>
-    <t>MOVE</t>
-  </si>
-  <si>
     <t>BRANCH</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>1001</t>
   </si>
   <si>
-    <t>STORE</t>
-  </si>
-  <si>
     <t>1010</t>
   </si>
   <si>
@@ -105,6 +96,12 @@
   </si>
   <si>
     <t>a(memory jump)</t>
+  </si>
+  <si>
+    <t>ADDI</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -140,13 +137,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +425,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="137" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:M8"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,7 +450,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -471,22 +469,22 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -496,23 +494,23 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>18</v>
+      <c r="A3" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -523,54 +521,57 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="N4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -578,28 +579,28 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -607,28 +608,28 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -636,28 +637,28 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -674,7 +675,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -688,17 +689,14 @@
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -712,17 +710,14 @@
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -737,10 +732,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -755,10 +750,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -773,10 +768,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -791,10 +786,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1222,39 +1217,44 @@
       <c r="P38" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="37">
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="F11:I11"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="F6:I6"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="N7:Q7"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J4:M4"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>